<commit_message>
added NJ data scraper
</commit_message>
<xml_diff>
--- a/sites.xlsx
+++ b/sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3586dc7e026dd77c/Documents/VSFS/Data scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{7D696CA8-DF62-4F83-B0E9-48DD79329F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48181F55-DAA3-4C3C-AAC9-6374D81B3ABC}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{7D696CA8-DF62-4F83-B0E9-48DD79329F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84E2E5C0-8C22-41BC-BF52-CBEFEF10E38F}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{4A848351-1019-41EE-B09A-C5773500E5C8}"/>
   </bookViews>
@@ -34,17 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>http://referral.unitedwayhouston.org/MatchList.aspx?c;;0;;N;0;0;Organizational/Community/International%20Services;Disaster%20Services;462;Extreme%20Heat%20Cooling%20Centers</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>https://centralusa.salvationarmy.org/midland/news/the-salvation-army-midland-division-opens-cooling-centers-with-missouri-and-illinois-to-battle-summer-heat/</t>
   </si>
   <si>
     <t>salvArmy</t>
   </si>
   <si>
-    <t>unitedWayHouston</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>https://web.archive.org/web/20210701183644/https://www.nj211.org/nj-cooling-centers</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20210619005125/https://centralusa.salvationarmy.org/midland/news/the-salvation-army-midland-division-opens-cooling-centers-with-missouri-and-illinois-to-battle-summer-heat/</t>
   </si>
 </sst>
 </file>
@@ -423,17 +417,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,29 +435,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D6C0CE1B-2827-40A7-888F-523ACC13E911}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{B89B3FF4-55B8-4D99-8613-4FD303462277}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B89B3FF4-55B8-4D99-8613-4FD303462277}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: moved classes into separate files
</commit_message>
<xml_diff>
--- a/sites.xlsx
+++ b/sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3586dc7e026dd77c/Documents/VSFS/Data scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{7D696CA8-DF62-4F83-B0E9-48DD79329F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84E2E5C0-8C22-41BC-BF52-CBEFEF10E38F}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{7D696CA8-DF62-4F83-B0E9-48DD79329F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{653C448D-4CC3-4DFC-835D-24122AA874BB}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{4A848351-1019-41EE-B09A-C5773500E5C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4A848351-1019-41EE-B09A-C5773500E5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://centralusa.salvationarmy.org/midland/news/the-salvation-army-midland-division-opens-cooling-centers-with-missouri-and-illinois-to-battle-summer-heat/</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>https://web.archive.org/web/20210701183644/https://www.nj211.org/nj-cooling-centers</t>
+  </si>
+  <si>
+    <t>unitedHouston</t>
+  </si>
+  <si>
+    <t>http://referral.unitedwayhouston.org/MatchList.aspx?c;;0;;N;0;0;Organizational/Community/International%20Services;Disaster%20Services;462;Extreme%20Heat%20Cooling%20Centers</t>
   </si>
 </sst>
 </file>
@@ -96,9 +102,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,7 +426,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,12 +456,19 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B89B3FF4-55B8-4D99-8613-4FD303462277}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{F5092E77-6B41-4DC7-BE12-B13BD9BA9977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>